<commit_message>
Impletmented Pwm, DIO, AIO robot model parts. Minor reorganization to match Arduino code.
</commit_message>
<xml_diff>
--- a/SerialDataFormat.xlsx
+++ b/SerialDataFormat.xlsx
@@ -4,22 +4,23 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="11475" windowHeight="5445" activeTab="5"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="11475" windowHeight="5445" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SerialPacketing" sheetId="1" r:id="rId1"/>
     <sheet name="IOCommandData" sheetId="2" r:id="rId2"/>
-    <sheet name="PWM(1)" sheetId="3" r:id="rId3"/>
-    <sheet name="DigitalIO" sheetId="4" r:id="rId4"/>
-    <sheet name="Encoder" sheetId="5" r:id="rId5"/>
-    <sheet name="AnalogIO" sheetId="6" r:id="rId6"/>
+    <sheet name="RSL(0)" sheetId="7" r:id="rId3"/>
+    <sheet name="PWM(1)" sheetId="3" r:id="rId4"/>
+    <sheet name="DigitalIO(2)" sheetId="4" r:id="rId5"/>
+    <sheet name="Encoder(4)" sheetId="5" r:id="rId6"/>
+    <sheet name="AnalogIO(3)" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
   <si>
     <t>Header</t>
   </si>
@@ -172,6 +173,12 @@
   </si>
   <si>
     <t>Number of sample to average, may not get implemented</t>
+  </si>
+  <si>
+    <t>Each bit sit high if the respectiev pin state should be set or retreived</t>
+  </si>
+  <si>
+    <t>DIOInUse</t>
   </si>
 </sst>
 </file>
@@ -869,10 +876,24 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J42" sqref="J42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+      <selection activeCell="I26" sqref="I26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1029,12 +1050,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:F1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E18" sqref="E18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1073,7 +1094,7 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C3" t="s">
         <v>10</v>
@@ -1085,41 +1106,50 @@
         <v>0</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A4" s="6"/>
-      <c r="B4" s="7" t="s">
-        <v>34</v>
-      </c>
-      <c r="C4" s="7" t="s">
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+      <c r="C4" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="7">
+      <c r="D4">
         <v>4</v>
       </c>
       <c r="E4" s="7">
         <v>4</v>
       </c>
-      <c r="F4" s="7" t="s">
+      <c r="F4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="6"/>
+      <c r="B5" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="C5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="7">
+        <v>4</v>
+      </c>
+      <c r="E5" s="7">
+        <v>8</v>
+      </c>
+      <c r="F5" s="7" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-    </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6" s="8"/>
-      <c r="B6" s="8"/>
-      <c r="C6" s="8"/>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="8"/>
@@ -1168,6 +1198,19 @@
       <c r="D12" s="8"/>
       <c r="E12" s="8"/>
       <c r="F12" s="8"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A13" s="8"/>
+      <c r="B13" s="8"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.25">
+      <c r="E18">
+        <v>2</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1177,12 +1220,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:F15"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1399,11 +1442,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
DIO and analog model sections impletmented on arduino Delayed initialization of secions on Arduino impletmented Moved some .net projects Configured all .net projects to output to shared directory
</commit_message>
<xml_diff>
--- a/SerialDataFormat.xlsx
+++ b/SerialDataFormat.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="75" windowWidth="11475" windowHeight="5445" firstSheet="2" activeTab="4"/>
+    <workbookView xWindow="240" yWindow="75" windowWidth="11475" windowHeight="5445" firstSheet="4" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="SerialPacketing" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="54">
   <si>
     <t>Header</t>
   </si>
@@ -179,6 +179,9 @@
   </si>
   <si>
     <t>DIOInUse</t>
+  </si>
+  <si>
+    <t>Staet</t>
   </si>
 </sst>
 </file>
@@ -876,14 +879,137 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="J42" sqref="J42"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="4.28515625" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="5.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" s="12" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" s="12"/>
+      <c r="C1" s="12"/>
+      <c r="D1" s="12"/>
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2" t="s">
+        <v>5</v>
+      </c>
+      <c r="E2" t="s">
+        <v>4</v>
+      </c>
+      <c r="F2" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>53</v>
+      </c>
+      <c r="C3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A4" s="4"/>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A5" s="4"/>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A6" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A8" s="4"/>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A9" s="8"/>
+      <c r="B9" s="8"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A10" s="4"/>
+      <c r="B10" s="4"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="4"/>
+      <c r="E10" s="4"/>
+      <c r="F10" s="4"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A11" s="4"/>
+      <c r="B11" s="4"/>
+      <c r="C11" s="4"/>
+      <c r="D11" s="4"/>
+      <c r="E11" s="4"/>
+      <c r="F11" s="4"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12" s="4"/>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -893,7 +1019,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I26" sqref="I26"/>
+      <selection activeCell="I26" sqref="A1:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1055,7 +1181,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>